<commit_message>
changes in file API
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,12 +565,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>02 Shaadi Shud I By Mohammed Hussain</t>
+          <t>01 Life ka Tamasha by Amandeep Khayal - Delhi</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Sun 6 Jul 2025</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -580,42 +580,42 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1 hour 30 minutes</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>12yrs+</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Hindi, English</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Aiwan-E-Ghalib Auditorium: Delhi</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>₹799 Onwards</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Fast Filling</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>02_Shaadi Shud I By Mohammed Hussain.png</t>
+          <t>01_Life ka Tamasha by Amandeep Khayal - Delhi.png</t>
         </is>
       </c>
     </row>
@@ -627,27 +627,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>03 Sufi Night ft. Sultani Brothers</t>
+          <t>02 Pottery Painting</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sun 22 Jun 2025</t>
+          <t>Sat 21 Jun 2025</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Sun 29 Jun 2025</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>8:00 PM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2 hours 30 minutes</t>
+          <t>1 hour 30 minutes</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>₹199</t>
+          <t>₹599 Onwards</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>03_Sufi Night ft. Sultani Brothers.png</t>
+          <t>02_Pottery Painting.png</t>
         </is>
       </c>
     </row>
@@ -689,12 +689,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>04 Sip and Paint - Mug Painting</t>
+          <t>02 Shaadi Shud I By Mohammed Hussain</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fri 18 Jul 2025</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -704,27 +704,27 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>5:00 PM</t>
+          <t>-</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1 hour 30 minutes</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>12yrs+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>BR English, Hindi</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Soaked in Canvas: Gurugram</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -734,12 +734,12 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>-</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>04_Sip and Paint - Mug Painting.png</t>
+          <t>02_Shaadi Shud I By Mohammed Hussain.png</t>
         </is>
       </c>
     </row>
@@ -751,57 +751,57 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>05 Kaviraj Singh LIVE!!!</t>
+          <t>03 Sufi Night ft. Sultani Brothers</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sat 21 Jun 2025</t>
+          <t>Sun 22 Jun 2025</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sat 5 Jul 2025</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>6:00 PM</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1 hour 15 minutes</t>
+          <t>2 hours 30 minutes</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>18yrs+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Hindi, English</t>
+          <t>-</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Comedy County: Noida</t>
+          <t>-</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>₹449 Onwards</t>
+          <t>₹199</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Fast Filling</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>05_Kaviraj Singh LIVE!!!.png</t>
+          <t>03_Sufi Night ft. Sultani Brothers.png</t>
         </is>
       </c>
     </row>
@@ -813,27 +813,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>06 STAND UP COMEDY SHOW</t>
+          <t>03 Vipul Goyal-Unleashed</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Wed 18 Jun 2025</t>
+          <t>Sun 22 Jun 2025</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Wed 9 Jul 2025</t>
+          <t>Sun 13 Jul 2025</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>8:30 PM</t>
+          <t>5:15 PM</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2 Hours</t>
+          <t>1 hour 15 minutes</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -848,22 +848,22 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Xero Degrees: Gurgaon</t>
+          <t>Studio XO Bar, Sector 29: Gurugram</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>₹149 Onwards</t>
+          <t>₹899 Onwards</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Fast Filling</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>06_STAND UP COMEDY SHOW.png</t>
+          <t>03_Vipul Goyal-Unleashed.png</t>
         </is>
       </c>
     </row>
@@ -875,42 +875,42 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>07 BLUNT ft. Onkar</t>
+          <t>04 Sip and Paint - Mug Painting</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Wed 18 Jun 2025</t>
+          <t>Fri 18 Jul 2025</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Sun 6 Jul 2025</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>8:00 PM</t>
+          <t>5:00 PM</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1 Hour</t>
+          <t>1 hour 30 minutes</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>16yrs+</t>
+          <t>12yrs+</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Hindi</t>
+          <t>BQ English, Hindi</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>The J Spot, Juhu: Mumbai</t>
+          <t>Soaked in Canvas: Gurugram</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -920,12 +920,12 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Fast Filling</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>07_BLUNT ft. Onkar.png</t>
+          <t>04_Sip and Paint - Mug Painting.png</t>
         </is>
       </c>
     </row>
@@ -937,42 +937,42 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>08 Hand Built Pottery</t>
+          <t>04 SONU NIGAM LIVE IN CONCERT GURUGRAM</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Tue 17 Jun 2025</t>
+          <t>Sat 1 Nov 2025</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Sat 5 Jul 2025</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>7:00 PM</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1 Hour</t>
+          <t>2 hours 30 minutes</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>5yrs+</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Bengali, English, Hindi, Kannada,</t>
+          <t>Hindi</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>@ Tiny House Cafe: Indore</t>
+          <t>Gymkhana Club: Gurugram</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -982,12 +982,12 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Fast Filling</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>08_Hand Built Pottery.png</t>
+          <t>04_SONU NIGAM LIVE IN CONCERT GURUGRAM.png</t>
         </is>
       </c>
     </row>
@@ -999,47 +999,47 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>09 Rahgir  Kya Jaipur Kya Dilli Tour</t>
+          <t>05 Halki Halki Fati By Vikas Kush Sharma</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sat 21 Jun 2025</t>
+          <t>Fri 20 Jun 2025</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Sat 12 Jul 2025</t>
+          <t>Sun 7 Sep 2025</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>5:30 PM</t>
+          <t>7:30 PM</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2 Hours</t>
+          <t>1 hour 30 minutes</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>12yrs+</t>
+          <t>16yrs+</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Hindi, English</t>
+          <t>English, Hindi</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Mehendi Navaz Jung Hall: q</t>
+          <t>Baroda Productivity Council</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>₹499 Onwards</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1049,7 +1049,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>09_Rahgir  Kya Jaipur Kya Dilli Tour.png</t>
+          <t>05_Halki Halki Fati By Vikas Kush Sharma.png</t>
         </is>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10 Texture Art ft. ChalkBooard</t>
+          <t>05 Kaviraj Singh LIVE!!!</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1071,47 +1071,47 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Sat 5 Jul 2025</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>11:30 AM</t>
+          <t>6:00 PM</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1 hour 30 minutes</t>
+          <t>1 hour 15 minutes</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>18yrs+</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Hindi, English</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Comedy County: Noida</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>₹599 Onwards</t>
+          <t>₹449 Onwards</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Fast Filling</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>10_Texture Art ft. ChalkBooard.png</t>
+          <t>05_Kaviraj Singh LIVE!!!.png</t>
         </is>
       </c>
     </row>
@@ -1123,17 +1123,17 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11 TELLING LIES-A STANDUP SOLO BY AASHISH SOLANKI</t>
+          <t>06 Comedy Nights Noida</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Sat 21 Jun 2025</t>
+          <t>Mon 16 Jun 2025</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Sun 27 Jul 2025</t>
+          <t>Tue 1 Jul 2025</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>1 hour 30 minutes</t>
+          <t>1 hour 15 minutes</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1153,17 +1153,17 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>English, Hindi</t>
+          <t>Hindi</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Y.B. Chavan Auditorium: Mumbai</t>
+          <t>Comedy County: Noida</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>₹499 Onwards</t>
+          <t>₹299 Onwards</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1173,7 +1173,7 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>11_TELLING LIES-A STANDUP SOLO BY AASHISH SOLANKI.png</t>
+          <t>06_Comedy Nights Noida.png</t>
         </is>
       </c>
     </row>
@@ -1185,27 +1185,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12 PS - I Love You By Pranav Sharma</t>
+          <t>06 STAND UP COMEDY SHOW</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Sat 21 Jun 2025</t>
+          <t>Wed 18 Jun 2025</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Sun 27 Jul 2025</t>
+          <t>Wed 9 Jul 2025</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2:00 PM</t>
+          <t>8:30 PM</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>1 hour 15 minutes</t>
+          <t>2 Hours</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1220,22 +1220,22 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Mysore Association Auditorium</t>
+          <t>Xero Degrees: Gurgaon</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>₹149 Onwards</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Fast Filling</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>12_PS - I Love You By Pranav Sharma.png</t>
+          <t>06_STAND UP COMEDY SHOW.png</t>
         </is>
       </c>
     </row>
@@ -1247,57 +1247,57 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>13 Pottery Workshop</t>
+          <t>07 BLUNT ft. Onkar</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Sat 21 Jun 2025</t>
+          <t>Wed 18 Jun 2025</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Sun 29 Jun 2025</t>
+          <t>Sun 6 Jul 2025</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>8:00 PM</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1 hour 30 minutes</t>
+          <t>1 Hour</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>16yrs+</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Hindi</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>The J Spot, Juhu: Mumbai</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>₹499 Onwards</t>
+          <t>-</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Available</t>
+          <t>Fast Filling</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>13_Pottery Workshop.png</t>
+          <t>07_BLUNT ft. Onkar.png</t>
         </is>
       </c>
     </row>
@@ -1309,57 +1309,1235 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>07 Young Adult! ft.Gurleen Pannu</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Fri 4 Jul 2025</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Sun 24 Aug 2025</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>6:00 PM</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>1 hour 15 minutes</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Hindi, English</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Y.B. Chavan Auditorium: Mumbai</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>₹499</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>07_Young Adult! ft.Gurleen Pannu.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>#0015</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>08 Hand Built Pottery</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Tue 17 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Sat 5 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>1 Hour</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Bengali, English, Hindi, Kannada,</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>@ Tiny House Cafe: Indore</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>₹499 Onwards</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>08_Hand Built Pottery.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>#0016</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>08 The Lineup ft. Gourav, Himanshu, Inder &amp; Pawan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Mon 16 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>9:30 PM</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>18yrs+</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Hindi, English</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>The Laugh Store: DLF Cyberhub</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>₹399 Onwards</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>08_The Lineup ft. Gourav, Himanshu, Inder &amp; Pawan.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>#0017</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>09 Rahgir  Kya Jaipur Kya Dilli Tour</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Sat 21 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Sat 12 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>5:30 PM</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2Hours</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>12yrs+</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Hindi, English</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Mehendi Navaz Jung Hall: V</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>₹499 Onwards</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Fast Filling</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>09_Rahgir  Kya Jaipur Kya Dilli Tour.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>#0018</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>09 The Duo ft. Harsh Gujral &amp; Rahul Dua</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Mon 23 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>7:00 PM</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>18yrs+</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>English, Hindi</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>The Laugh Store: DLF Cyberhub</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>₹799 Onwards</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Fast Filling</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>09_The Duo ft. Harsh Gujral &amp; Rahul Dua.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>#0019</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>10 ALLOW ME - A Standup Comedy Show by Rahul Dua</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Fri 20 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Hindi, English</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>The Laugh Store: DLF Cyberhub</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>₹499 Onwards</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Fast Filling</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>10_ALLOW ME - A Standup Comedy Show by Rahul Dua.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>#0020</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>10 Texture Art ft. ChalkBooard</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sat 21 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>11:30 AM</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>₹599 Onwards</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>10_Texture Art ft. ChalkBooard.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>#0021</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11 Moon Lamp workshop</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Tue 17 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Sun 13 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2Hours</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>₹799 Onwards</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>11_Moon Lamp workshop.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>#0022</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>11 TELLING LIES-A STANDUP SOLO BY AASHISH SOLANKI</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Sat 21 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Sun 27 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>9:00 PM</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>English, Hindi</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Y.B. Chavan Auditorium: Mumbai</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>₹499 Onwards</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>11_TELLING LIES-A STANDUP SOLO BY AASHISH SOLANKI.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>#0023</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>12 Open Mic</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Mon 16 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Tue 17 Jun 2025</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>5:00 PM</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Hindi, English</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>The Laugh Store: DLF Cyberhub</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>₹299</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>12_Open Mic.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>#0024</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>12 PS - I Love You By Pranav Sharma</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Sat 21 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Sun 27 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>2:00 PM</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>1 hour 15 minutes</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Hindi, English</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Mysore Association Auditorium</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Fast Filling</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>12_PS - I Love You By Pranav Sharma.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>#0025</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>13 Kisi Ko Batana Mat By Anubhav Singh Bassi</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Thu 26 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>9:00PM</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2hours 15 minutes</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Hindi</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>The Laugh Store: DLF Cyberhub</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>₹499</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>13_Kisi Ko Batana Mat By Anubhav Singh Bassi.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>#0026</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>13 Pottery Workshop</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Sat 21 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Sun 29 Jun 2025</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>₹499 Onwards</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>13_Pottery Workshop.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>#0027</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>14 Meet the Dinosaurs at North India Mall</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Tue 17 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Mon 30 Jun 2025</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>12:00 PM</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>9 Hours</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>₹99 Onwards</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>14_Meet the Dinosaurs at North India Mall.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>#0028</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>14 Standup Stars - The Best of Stand-Up</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>Tue 17 Jun 2025</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Sat 12 Jul 2025</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>8:00 PM</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>1 hour 20 minutes</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>18yrs+</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>English, Hindi</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t>Laughter Nation Comedy Club</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>₹249 Onwards</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr">
+      <c r="K29" t="inlineStr">
         <is>
           <t>Available</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="L29" t="inlineStr">
         <is>
           <t>14_Standup Stars - The Best of Stand-Up.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>#0029</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>15 Comedy Nights @Comedy County</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Mon 16 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Thu 3 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>9:00 PM</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1 hour 15 minutes</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Hindi</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Comedy County: Noida</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>₹299 Onwards</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>15_Comedy Nights @Comedy County.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>#0030</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16 The Lineup ft. Chirag, Pranav, Kaustubh &amp; Vivek</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>16_The Lineup ft. Chirag, Pranav, Kaustubh &amp; Vivek.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>#0031</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>17 Tum, Main aur Ishq - Ashish Bagrecha</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Sat 21 Jun 2025</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Sun 20 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>7:00 PM</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2 Hours</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>₹499 Onwards</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Fast Filling</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>17_Tum, Main aur Ishq - Ashish Bagrecha.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>#0032</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>18 Best of Laugh Store ft. Manik, Maheep &amp; Swati</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Tue 1 Jul 2025</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Thu 3 Jul 2025</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>9:30 PM</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>18yrs+</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>@3_ Hindi, English</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>The Laugh Store: DLF Cyberhub</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>₹599</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>18_Best of Laugh Store ft. Manik, Maheep &amp; Swati.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>#0033</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>19 Mauka Ya Dhoka Ft. Inder Sahani</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Fri 25 Jul 2025</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>9:30 PM</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>1 hour 30 minutes</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>16yrs+</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Hindi, English</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>The Laugh Store: DLF Cyberhub</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>₹399 Onwards</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>19_Mauka Ya Dhoka Ft. Inder Sahani.png</t>
         </is>
       </c>
     </row>

</xml_diff>